<commit_message>
corrected filepath for income_counts_entry_and_exit function
</commit_message>
<xml_diff>
--- a/BoSClean/Income Counts Entry and Exit.xlsx
+++ b/BoSClean/Income Counts Entry and Exit.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Income Counts Entry and Exit" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>294</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11486</v>
+        <v>17</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>342</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -531,7 +531,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12210</v>
+        <v>18</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>11495</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4783</v>
+        <v>1834</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>197</v>
+        <v>102</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5076</v>
+        <v>1855</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>315</v>
+        <v>52</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12265</v>
+        <v>2621</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>323</v>
+        <v>154</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -771,7 +771,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12613</v>
+        <v>2958</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -791,7 +791,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>143</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1193</v>
+        <v>5417</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -851,7 +851,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1208</v>
+        <v>5668</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>581</v>
+        <v>75</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>610</v>
+        <v>90</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Erin Park</t>
+          <t>Erin</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1237</v>
+        <v>697</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1253</v>
+        <v>713</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MC PATH</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2373</v>
+        <v>978</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2387</v>
+        <v>995</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>OC PATH</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>893</v>
+        <v>71</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>887</v>
+        <v>72</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>

</xml_diff>